<commit_message>
heatmap file variable sequence changed
</commit_message>
<xml_diff>
--- a/heatmap.xlsx
+++ b/heatmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammadnaumanshahid/Downloads/chord_diagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021F63E0-F07F-EF4A-8A28-0112CB31FAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDBF44A-49BB-6B49-8391-624CB7032848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{CA20361F-4654-354D-ACE8-71BF32DD6564}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -399,16 +399,16 @@
         <v>0.72</v>
       </c>
       <c r="C1" s="1">
-        <v>-0.04</v>
+        <v>-0.09</v>
       </c>
       <c r="D1" s="1">
-        <v>-0.09</v>
+        <v>-0.03</v>
       </c>
       <c r="E1" s="1">
-        <v>-0.03</v>
+        <v>0.03</v>
       </c>
       <c r="F1" s="1">
-        <v>0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="G1" s="1">
         <v>-0.02</v>
@@ -423,16 +423,16 @@
         <v>0.08</v>
       </c>
       <c r="K1" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="L1" s="1">
         <v>-0.08</v>
       </c>
-      <c r="L1" s="1">
-        <v>-0.04</v>
-      </c>
       <c r="M1" s="1">
-        <v>-0.02</v>
+        <v>-0.04</v>
       </c>
       <c r="N1" s="1">
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="O1" s="1">
         <v>-0.03</v>
@@ -441,10 +441,10 @@
         <v>-0.02</v>
       </c>
       <c r="Q1" s="1">
-        <v>-0.01</v>
+        <v>-0.03</v>
       </c>
       <c r="R1" s="1">
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="S1" s="1">
         <v>-0.01</v>
@@ -453,13 +453,13 @@
         <v>-0.02</v>
       </c>
       <c r="U1" s="1">
-        <v>-0.04</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="V1" s="1">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.01</v>
       </c>
       <c r="W1" s="1">
-        <v>-0.01</v>
+        <v>-0.04</v>
       </c>
       <c r="X1" s="1">
         <v>-0.02</v>
@@ -479,16 +479,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
+        <v>-0.12</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="F2" s="1">
         <v>-0.08</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-0.12</v>
-      </c>
-      <c r="E2" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.03</v>
       </c>
       <c r="G2" s="1">
         <v>-0.04</v>
@@ -503,28 +503,28 @@
         <v>0.08</v>
       </c>
       <c r="K2" s="1">
-        <v>-0.04</v>
+        <v>0.01</v>
       </c>
       <c r="L2" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="M2" s="1">
         <v>0.06</v>
       </c>
-      <c r="M2" s="1">
-        <v>-0.05</v>
-      </c>
       <c r="N2" s="1">
-        <v>-0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="O2" s="1">
-        <v>0.01</v>
+        <v>-0.03</v>
       </c>
       <c r="P2" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q2" s="1">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
       <c r="R2" s="1">
-        <v>-0.03</v>
+        <v>0.03</v>
       </c>
       <c r="S2" s="1">
         <v>0.02</v>
@@ -533,13 +533,13 @@
         <v>-0.01</v>
       </c>
       <c r="U2" s="1">
-        <v>-0.04</v>
+        <v>-0.09</v>
       </c>
       <c r="V2" s="1">
-        <v>-0.09</v>
+        <v>-0.01</v>
       </c>
       <c r="W2" s="1">
-        <v>-0.01</v>
+        <v>-0.04</v>
       </c>
       <c r="X2" s="1">
         <v>-0.03</v>
@@ -553,322 +553,322 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>-0.04</v>
+        <v>-0.09</v>
       </c>
       <c r="B3" s="1">
-        <v>-0.08</v>
+        <v>-0.12</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1">
+        <v>-0.06</v>
+      </c>
+      <c r="E3" s="1">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="E3" s="1">
-        <v>0.37</v>
-      </c>
       <c r="F3" s="1">
-        <v>0.24</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>0.02</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>-0.01</v>
+        <v>-0.05</v>
       </c>
       <c r="I3" s="1">
-        <v>0.12</v>
+        <v>-0.05</v>
       </c>
       <c r="J3" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>-0.04</v>
       </c>
       <c r="K3" s="1">
+        <v>-0.09</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="M3" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="O3" s="1">
         <v>0.04</v>
       </c>
-      <c r="L3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="O3" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
       <c r="P3" s="1">
-        <v>0.01</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="Q3" s="1">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="R3" s="1">
-        <v>0.1</v>
+        <v>-0.04</v>
       </c>
       <c r="S3" s="1">
-        <v>-0.04</v>
+        <v>0.03</v>
       </c>
       <c r="T3" s="1">
-        <v>0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="U3" s="1">
-        <v>0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="V3" s="1">
-        <v>0.83</v>
+        <v>-0.02</v>
       </c>
       <c r="W3" s="1">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="X3" s="1">
-        <v>0</v>
+        <v>-0.02</v>
       </c>
       <c r="Y3" s="1">
         <v>0</v>
       </c>
       <c r="Z3" s="1">
-        <v>0.04</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>-0.09</v>
+        <v>-0.03</v>
       </c>
       <c r="B4" s="1">
-        <v>-0.12</v>
+        <v>-0.04</v>
       </c>
       <c r="C4" s="1">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.06</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>-0.06</v>
+        <v>0.03</v>
       </c>
       <c r="F4" s="1">
-        <v>-7.0000000000000007E-2</v>
+        <v>0.37</v>
       </c>
       <c r="G4" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>-0.02</v>
       </c>
       <c r="H4" s="1">
-        <v>-0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I4" s="1">
-        <v>-0.05</v>
+        <v>0.03</v>
       </c>
       <c r="J4" s="1">
-        <v>-0.04</v>
+        <v>0.01</v>
       </c>
       <c r="K4" s="1">
-        <v>0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="L4" s="1">
         <v>-0.05</v>
       </c>
       <c r="M4" s="1">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
       <c r="N4" s="1">
-        <v>0.04</v>
+        <v>-0.04</v>
       </c>
       <c r="O4" s="1">
-        <v>-0.09</v>
+        <v>-0.03</v>
       </c>
       <c r="P4" s="1">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.04</v>
       </c>
       <c r="Q4" s="1">
-        <v>-0.04</v>
+        <v>-0.03</v>
       </c>
       <c r="R4" s="1">
-        <v>0.17</v>
+        <v>-0.04</v>
       </c>
       <c r="S4" s="1">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="T4" s="1">
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="U4" s="1">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="V4" s="1">
         <v>-0.02</v>
       </c>
       <c r="W4" s="1">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="X4" s="1">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="Y4" s="1">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="Z4" s="1">
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>-0.03</v>
+        <v>0.03</v>
       </c>
       <c r="B5" s="1">
-        <v>-0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C5" s="1">
-        <v>0.37</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D5" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="L5" s="1">
+        <v>-0.02</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="N5" s="1">
+        <v>-0.02</v>
+      </c>
+      <c r="O5" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
         <v>-0.06</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="G5" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="K5" s="1">
-        <v>-0.05</v>
-      </c>
-      <c r="L5" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="M5" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="N5" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="O5" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="P5" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>-0.04</v>
-      </c>
       <c r="R5" s="1">
-        <v>-0.03</v>
+        <v>0.05</v>
       </c>
       <c r="S5" s="1">
-        <v>-0.05</v>
+        <v>0.01</v>
       </c>
       <c r="T5" s="1">
-        <v>-0.01</v>
+        <v>0.01</v>
       </c>
       <c r="U5" s="1">
-        <v>-0.03</v>
+        <v>0.22</v>
       </c>
       <c r="V5" s="1">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="W5" s="1">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="X5" s="1">
-        <v>-0.01</v>
+        <v>-0.03</v>
       </c>
       <c r="Y5" s="1">
-        <v>-0.01</v>
+        <v>-0.05</v>
       </c>
       <c r="Z5" s="1">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="B6" s="1">
-        <v>0.03</v>
+        <v>-0.08</v>
       </c>
       <c r="C6" s="1">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="E6" s="1">
         <v>0.24</v>
       </c>
-      <c r="D6" s="1">
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.03</v>
-      </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H6" s="1">
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="I6" s="1">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
       <c r="J6" s="1">
-        <v>0.16</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K6" s="1">
-        <v>-0.02</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L6" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="T6" s="1">
         <v>0.05</v>
       </c>
-      <c r="M6" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="N6" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="R6" s="1">
-        <v>-0.06</v>
-      </c>
-      <c r="S6" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="T6" s="1">
-        <v>0.01</v>
-      </c>
       <c r="U6" s="1">
-        <v>-0.03</v>
+        <v>0.83</v>
       </c>
       <c r="V6" s="1">
-        <v>0.22</v>
+        <v>0.08</v>
       </c>
       <c r="W6" s="1">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="X6" s="1">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="1">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -879,16 +879,16 @@
         <v>-0.04</v>
       </c>
       <c r="C7" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-0.02</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F7" s="1">
         <v>0.02</v>
-      </c>
-      <c r="D7" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.01</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -903,28 +903,28 @@
         <v>0.1</v>
       </c>
       <c r="K7" s="1">
-        <v>-0.05</v>
+        <v>-0.06</v>
       </c>
       <c r="L7" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="M7" s="1">
         <v>-0.06</v>
       </c>
-      <c r="M7" s="1">
-        <v>-0.04</v>
-      </c>
       <c r="N7" s="1">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="O7" s="1">
-        <v>-0.06</v>
+        <v>-0.03</v>
       </c>
       <c r="P7" s="1">
         <v>-0.06</v>
       </c>
       <c r="Q7" s="1">
-        <v>-0.04</v>
+        <v>-0.01</v>
       </c>
       <c r="R7" s="1">
-        <v>-0.01</v>
+        <v>-0.04</v>
       </c>
       <c r="S7" s="1">
         <v>-0.06</v>
@@ -933,13 +933,13 @@
         <v>0</v>
       </c>
       <c r="U7" s="1">
-        <v>-0.03</v>
+        <v>0.02</v>
       </c>
       <c r="V7" s="1">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="W7" s="1">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
       <c r="X7" s="1">
         <v>-0.02</v>
@@ -959,16 +959,16 @@
         <v>0.11</v>
       </c>
       <c r="C8" s="1">
-        <v>-0.01</v>
+        <v>-0.05</v>
       </c>
       <c r="D8" s="1">
-        <v>-0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E8" s="1">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
       <c r="F8" s="1">
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="G8" s="1">
         <v>-0.02</v>
@@ -983,28 +983,28 @@
         <v>0.03</v>
       </c>
       <c r="K8" s="1">
-        <v>-0.01</v>
+        <v>-0.05</v>
       </c>
       <c r="L8" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="M8" s="1">
         <v>0.04</v>
       </c>
-      <c r="M8" s="1">
-        <v>-0.04</v>
-      </c>
       <c r="N8" s="1">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="O8" s="1">
-        <v>-0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="P8" s="1">
         <v>-0.02</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.01</v>
+        <v>0.13</v>
       </c>
       <c r="R8" s="1">
-        <v>0.13</v>
+        <v>0.01</v>
       </c>
       <c r="S8" s="1">
         <v>-0.01</v>
@@ -1013,13 +1013,13 @@
         <v>0</v>
       </c>
       <c r="U8" s="1">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="V8" s="1">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="W8" s="1">
-        <v>-0.04</v>
+        <v>-0.02</v>
       </c>
       <c r="X8" s="1">
         <v>-0.01</v>
@@ -1039,16 +1039,16 @@
         <v>0</v>
       </c>
       <c r="C9" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="F9" s="1">
         <v>0.12</v>
-      </c>
-      <c r="D9" s="1">
-        <v>-0.05</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.06</v>
       </c>
       <c r="G9" s="1">
         <v>0.1</v>
@@ -1063,28 +1063,28 @@
         <v>0.09</v>
       </c>
       <c r="K9" s="1">
-        <v>-0.04</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="M9" s="1">
         <v>-0.08</v>
       </c>
-      <c r="M9" s="1">
-        <v>-0.05</v>
-      </c>
       <c r="N9" s="1">
         <v>-0.05</v>
       </c>
       <c r="O9" s="1">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="P9" s="1">
         <v>-0.06</v>
       </c>
       <c r="Q9" s="1">
-        <v>-0.04</v>
+        <v>-0.03</v>
       </c>
       <c r="R9" s="1">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="S9" s="1">
         <v>-0.05</v>
@@ -1093,13 +1093,13 @@
         <v>0.01</v>
       </c>
       <c r="U9" s="1">
-        <v>-0.04</v>
+        <v>0.1</v>
       </c>
       <c r="V9" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="W9" s="1">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="X9" s="1">
         <v>-0.02</v>
@@ -1119,16 +1119,16 @@
         <v>0.08</v>
       </c>
       <c r="C10" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="F10" s="1">
         <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.16</v>
       </c>
       <c r="G10" s="1">
         <v>0.1</v>
@@ -1143,28 +1143,28 @@
         <v>1</v>
       </c>
       <c r="K10" s="1">
-        <v>-0.04</v>
+        <v>-0.01</v>
       </c>
       <c r="L10" s="1">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="M10" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="N10" s="1">
         <v>-0.06</v>
       </c>
-      <c r="N10" s="1">
-        <v>-0.05</v>
-      </c>
       <c r="O10" s="1">
-        <v>-0.01</v>
+        <v>-0.05</v>
       </c>
       <c r="P10" s="1">
         <v>-0.05</v>
       </c>
       <c r="Q10" s="1">
-        <v>-0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="R10" s="1">
-        <v>-0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="S10" s="1">
         <v>-0.02</v>
@@ -1173,13 +1173,13 @@
         <v>-0.02</v>
       </c>
       <c r="U10" s="1">
-        <v>-0.05</v>
+        <v>0.06</v>
       </c>
       <c r="V10" s="1">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="W10" s="1">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="X10" s="1">
         <v>-0.03</v>
@@ -1193,200 +1193,200 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>-0.08</v>
+        <v>-0.03</v>
       </c>
       <c r="B11" s="1">
-        <v>-0.04</v>
+        <v>0.01</v>
       </c>
       <c r="C11" s="1">
+        <v>-0.09</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-0.06</v>
+      </c>
+      <c r="H11" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="N11" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="O11" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="P11" s="1">
         <v>0.04</v>
       </c>
-      <c r="D11" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="E11" s="1">
-        <v>-0.05</v>
-      </c>
-      <c r="F11" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="G11" s="1">
-        <v>-0.05</v>
-      </c>
-      <c r="H11" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="I11" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="J11" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="K11" s="1">
-        <v>1</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="M11" s="1">
+      <c r="Q11" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="U11" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N11" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="O11" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="P11" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>0</v>
-      </c>
-      <c r="R11" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="S11" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="T11" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="U11" s="1">
-        <v>0.03</v>
-      </c>
       <c r="V11" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="W11" s="1">
         <v>0.06</v>
       </c>
-      <c r="W11" s="1">
-        <v>0.02</v>
-      </c>
       <c r="X11" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="Y11" s="1">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="Z11" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>-0.04</v>
+        <v>-0.08</v>
       </c>
       <c r="B12" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-0.02</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="H12" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="I12" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="N12" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="U12" s="1">
         <v>0.06</v>
       </c>
-      <c r="C12" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-0.05</v>
-      </c>
-      <c r="E12" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="G12" s="1">
-        <v>-0.06</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="I12" s="1">
-        <v>-0.08</v>
-      </c>
-      <c r="J12" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="K12" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="L12" s="1">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="N12" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="O12" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="P12" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="R12" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="S12" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="T12" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="U12" s="1">
-        <v>0</v>
-      </c>
       <c r="V12" s="1">
-        <v>0.09</v>
+        <v>0.02</v>
       </c>
       <c r="W12" s="1">
-        <v>-0.04</v>
+        <v>0.03</v>
       </c>
       <c r="X12" s="1">
-        <v>-0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="Y12" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="Z12" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>-0.02</v>
+        <v>-0.04</v>
       </c>
       <c r="B13" s="1">
-        <v>-0.05</v>
+        <v>0.06</v>
       </c>
       <c r="C13" s="1">
-        <v>0.02</v>
+        <v>-0.05</v>
       </c>
       <c r="D13" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-0.06</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="I13" s="1">
+        <v>-0.08</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="K13" s="1">
         <v>0.09</v>
       </c>
-      <c r="E13" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="F13" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="G13" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="H13" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="I13" s="1">
-        <v>-0.05</v>
-      </c>
-      <c r="J13" s="1">
-        <v>-0.06</v>
-      </c>
-      <c r="K13" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
       <c r="L13" s="1">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="M13" s="1">
         <v>1</v>
@@ -1395,78 +1395,78 @@
         <v>0.1</v>
       </c>
       <c r="O13" s="1">
-        <v>-0.04</v>
+        <v>0.13</v>
       </c>
       <c r="P13" s="1">
-        <v>-0.01</v>
+        <v>0.13</v>
       </c>
       <c r="Q13" s="1">
         <v>-0.01</v>
       </c>
       <c r="R13" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="T13" s="1">
         <v>0.04</v>
       </c>
-      <c r="S13" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="T13" s="1">
-        <v>-0.01</v>
-      </c>
       <c r="U13" s="1">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
       <c r="V13" s="1">
-        <v>0.05</v>
+        <v>-0.04</v>
       </c>
       <c r="W13" s="1">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="X13" s="1">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="Y13" s="1">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="1">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="B14" s="1">
-        <v>-0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="C14" s="1">
-        <v>0.01</v>
+        <v>0.09</v>
       </c>
       <c r="D14" s="1">
-        <v>0.04</v>
+        <v>-0.04</v>
       </c>
       <c r="E14" s="1">
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="F14" s="1">
-        <v>-0.04</v>
+        <v>0.02</v>
       </c>
       <c r="G14" s="1">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="H14" s="1">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="I14" s="1">
         <v>-0.05</v>
       </c>
       <c r="J14" s="1">
-        <v>-0.05</v>
+        <v>-0.06</v>
       </c>
       <c r="K14" s="1">
-        <v>0.05</v>
+        <v>-0.04</v>
       </c>
       <c r="L14" s="1">
-        <v>0.13</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M14" s="1">
         <v>0.1</v>
@@ -1475,40 +1475,40 @@
         <v>1</v>
       </c>
       <c r="O14" s="1">
-        <v>-0.04</v>
+        <v>0.1</v>
       </c>
       <c r="P14" s="1">
-        <v>0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="Q14" s="1">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="R14" s="1">
-        <v>0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="S14" s="1">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="T14" s="1">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="U14" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="V14" s="1">
-        <v>0.05</v>
+        <v>-0.01</v>
       </c>
       <c r="W14" s="1">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="X14" s="1">
         <v>-0.02</v>
       </c>
       <c r="Y14" s="1">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="Z14" s="1">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
@@ -1516,76 +1516,76 @@
         <v>-0.03</v>
       </c>
       <c r="B15" s="1">
-        <v>0.01</v>
+        <v>-0.03</v>
       </c>
       <c r="C15" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D15" s="1">
-        <v>-0.09</v>
+        <v>-0.03</v>
       </c>
       <c r="E15" s="1">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="F15" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="H15" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="I15" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="J15" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="K15" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="Q15" s="1">
         <v>0.02</v>
       </c>
-      <c r="G15" s="1">
-        <v>-0.06</v>
-      </c>
-      <c r="H15" s="1">
-        <v>-0.05</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="L15" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="M15" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="N15" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="O15" s="1">
-        <v>1</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>0.19</v>
-      </c>
       <c r="R15" s="1">
-        <v>-0.01</v>
+        <v>0.01</v>
       </c>
       <c r="S15" s="1">
-        <v>0.11</v>
+        <v>0.01</v>
       </c>
       <c r="T15" s="1">
-        <v>0.09</v>
+        <v>0.01</v>
       </c>
       <c r="U15" s="1">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="V15" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="W15" s="1">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="X15" s="1">
-        <v>0.04</v>
+        <v>-0.02</v>
       </c>
       <c r="Y15" s="1">
-        <v>0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="Z15" s="1">
         <v>-0.01</v>
@@ -1599,16 +1599,16 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C16" s="1">
-        <v>0.01</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D16" s="1">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.04</v>
       </c>
       <c r="E16" s="1">
-        <v>-0.04</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G16" s="1">
         <v>-0.06</v>
@@ -1623,28 +1623,28 @@
         <v>-0.05</v>
       </c>
       <c r="K16" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="L16" s="1">
         <v>0.1</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M16" s="1">
         <v>0.13</v>
       </c>
-      <c r="M16" s="1">
-        <v>-0.01</v>
-      </c>
       <c r="N16" s="1">
-        <v>0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="O16" s="1">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="P16" s="1">
         <v>1</v>
       </c>
       <c r="Q16" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="R16" s="1">
         <v>0.05</v>
-      </c>
-      <c r="R16" s="1">
-        <v>-0.01</v>
       </c>
       <c r="S16" s="1">
         <v>0.06</v>
@@ -1653,10 +1653,10 @@
         <v>0.05</v>
       </c>
       <c r="U16" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="V16" s="1">
         <v>0.06</v>
-      </c>
-      <c r="V16" s="1">
-        <v>0.03</v>
       </c>
       <c r="W16" s="1">
         <v>0.06</v>
@@ -1673,132 +1673,132 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>-0.01</v>
+        <v>-0.03</v>
       </c>
       <c r="B17" s="1">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="D17" s="1">
-        <v>-0.04</v>
+        <v>-0.03</v>
       </c>
       <c r="E17" s="1">
-        <v>-0.04</v>
+        <v>-0.06</v>
       </c>
       <c r="F17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="I17" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="J17" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="K17" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="L17" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M17" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="P17" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>1</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="W17" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="X17" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="Z17" s="1">
         <v>0.05</v>
-      </c>
-      <c r="G17" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="I17" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="J17" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="M17" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="N17" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="O17" s="1">
-        <v>0.19</v>
-      </c>
-      <c r="P17" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>1</v>
-      </c>
-      <c r="R17" s="1">
-        <v>0</v>
-      </c>
-      <c r="S17" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="T17" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="U17" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="V17" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="W17" s="1">
-        <v>0</v>
-      </c>
-      <c r="X17" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="Y17" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="1">
-        <v>-0.04</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="B18" s="1">
-        <v>-0.03</v>
+        <v>0.03</v>
       </c>
       <c r="C18" s="1">
-        <v>0.1</v>
+        <v>-0.04</v>
       </c>
       <c r="D18" s="1">
-        <v>0.17</v>
+        <v>-0.04</v>
       </c>
       <c r="E18" s="1">
-        <v>-0.03</v>
+        <v>0.05</v>
       </c>
       <c r="F18" s="1">
-        <v>-0.06</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>-0.01</v>
+        <v>-0.04</v>
       </c>
       <c r="H18" s="1">
-        <v>0.13</v>
+        <v>0.01</v>
       </c>
       <c r="I18" s="1">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="J18" s="1">
-        <v>-0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="K18" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.19</v>
       </c>
       <c r="L18" s="1">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="M18" s="1">
-        <v>0.04</v>
+        <v>0.18</v>
       </c>
       <c r="N18" s="1">
-        <v>0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="O18" s="1">
-        <v>-0.01</v>
+        <v>0.01</v>
       </c>
       <c r="P18" s="1">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
       <c r="Q18" s="1">
         <v>0</v>
@@ -1807,28 +1807,28 @@
         <v>1</v>
       </c>
       <c r="S18" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.21</v>
       </c>
       <c r="T18" s="1">
-        <v>0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="U18" s="1">
-        <v>0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="V18" s="1">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="W18" s="1">
-        <v>0.17</v>
+        <v>-0.03</v>
       </c>
       <c r="X18" s="1">
-        <v>0.09</v>
+        <v>-0.02</v>
       </c>
       <c r="Y18" s="1">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="1">
-        <v>0.05</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
@@ -1839,16 +1839,16 @@
         <v>0.02</v>
       </c>
       <c r="C19" s="1">
-        <v>-0.04</v>
+        <v>0.03</v>
       </c>
       <c r="D19" s="1">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="E19" s="1">
-        <v>-0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F19" s="1">
-        <v>0.01</v>
+        <v>-0.04</v>
       </c>
       <c r="G19" s="1">
         <v>-0.06</v>
@@ -1863,28 +1863,28 @@
         <v>-0.02</v>
       </c>
       <c r="K19" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="L19" s="1">
         <v>0.08</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
         <v>0.06</v>
       </c>
-      <c r="M19" s="1">
-        <v>-0.01</v>
-      </c>
       <c r="N19" s="1">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="O19" s="1">
-        <v>0.11</v>
+        <v>0.01</v>
       </c>
       <c r="P19" s="1">
         <v>0.06</v>
       </c>
       <c r="Q19" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R19" s="1">
         <v>0.21</v>
-      </c>
-      <c r="R19" s="1">
-        <v>7.0000000000000007E-2</v>
       </c>
       <c r="S19" s="1">
         <v>1</v>
@@ -1893,13 +1893,13 @@
         <v>0.02</v>
       </c>
       <c r="U19" s="1">
-        <v>0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="V19" s="1">
         <v>-0.02</v>
       </c>
       <c r="W19" s="1">
-        <v>-0.02</v>
+        <v>0.01</v>
       </c>
       <c r="X19" s="1">
         <v>-0.01</v>
@@ -1919,17 +1919,17 @@
         <v>-0.01</v>
       </c>
       <c r="C20" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F20" s="1">
         <v>0.05</v>
       </c>
-      <c r="D20" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="E20" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0.01</v>
-      </c>
       <c r="G20" s="1">
         <v>0</v>
       </c>
@@ -1943,28 +1943,28 @@
         <v>-0.02</v>
       </c>
       <c r="K20" s="1">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="L20" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="M20" s="1">
         <v>0.04</v>
       </c>
-      <c r="M20" s="1">
-        <v>-0.01</v>
-      </c>
       <c r="N20" s="1">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="O20" s="1">
-        <v>0.09</v>
+        <v>0.01</v>
       </c>
       <c r="P20" s="1">
         <v>0.05</v>
       </c>
       <c r="Q20" s="1">
-        <v>-0.01</v>
+        <v>0.1</v>
       </c>
       <c r="R20" s="1">
-        <v>0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="S20" s="1">
         <v>0.02</v>
@@ -1973,13 +1973,13 @@
         <v>1</v>
       </c>
       <c r="U20" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="W20" s="1">
         <v>0.1</v>
-      </c>
-      <c r="V20" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="W20" s="1">
-        <v>0.11</v>
       </c>
       <c r="X20" s="1">
         <v>0.04</v>
@@ -1993,242 +1993,242 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>-0.04</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="B21" s="1">
-        <v>-0.04</v>
+        <v>-0.09</v>
       </c>
       <c r="C21" s="1">
-        <v>0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="E21" s="1">
-        <v>-0.03</v>
+        <v>0.22</v>
       </c>
       <c r="F21" s="1">
-        <v>-0.03</v>
+        <v>0.83</v>
       </c>
       <c r="G21" s="1">
-        <v>-0.03</v>
+        <v>0.02</v>
       </c>
       <c r="H21" s="1">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1">
-        <v>-0.04</v>
+        <v>0.1</v>
       </c>
       <c r="J21" s="1">
-        <v>-0.05</v>
+        <v>0.06</v>
       </c>
       <c r="K21" s="1">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L21" s="1">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="M21" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R21" s="1">
+        <v>-0.02</v>
+      </c>
+      <c r="S21" s="1">
+        <v>-0.02</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="U21" s="1">
+        <v>1</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="W21" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X21" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="Y21" s="1">
         <v>0.04</v>
       </c>
-      <c r="N21" s="1">
-        <v>0</v>
-      </c>
-      <c r="O21" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="P21" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="R21" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="S21" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="T21" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="U21" s="1">
-        <v>1</v>
-      </c>
-      <c r="V21" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="W21" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="X21" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="Y21" s="1">
-        <v>0.17</v>
-      </c>
       <c r="Z21" s="1">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.01</v>
       </c>
       <c r="B22" s="1">
-        <v>-0.09</v>
+        <v>-0.01</v>
       </c>
       <c r="C22" s="1">
-        <v>0.83</v>
+        <v>-0.02</v>
       </c>
       <c r="D22" s="1">
         <v>-0.02</v>
       </c>
       <c r="E22" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="H22" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="M22" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="N22" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
         <v>0.06</v>
       </c>
-      <c r="F22" s="1">
-        <v>0.22</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="J22" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="K22" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="L22" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="M22" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="N22" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="O22" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="P22" s="1">
-        <v>0.03</v>
-      </c>
       <c r="Q22" s="1">
-        <v>-0.02</v>
+        <v>0.17</v>
       </c>
       <c r="R22" s="1">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="S22" s="1">
         <v>-0.02</v>
       </c>
       <c r="T22" s="1">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="U22" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.12</v>
       </c>
       <c r="V22" s="1">
         <v>1</v>
       </c>
       <c r="W22" s="1">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="X22" s="1">
-        <v>0.03</v>
+        <v>0.33</v>
       </c>
       <c r="Y22" s="1">
-        <v>0.04</v>
+        <v>0.21</v>
       </c>
       <c r="Z22" s="1">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>-0.01</v>
+        <v>-0.04</v>
       </c>
       <c r="B23" s="1">
-        <v>-0.01</v>
+        <v>-0.04</v>
       </c>
       <c r="C23" s="1">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="E23" s="1">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="F23" s="1">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="G23" s="1">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
       <c r="H23" s="1">
-        <v>-0.04</v>
+        <v>-0.02</v>
       </c>
       <c r="I23" s="1">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="J23" s="1">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="K23" s="1">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="L23" s="1">
-        <v>-0.04</v>
+        <v>0.03</v>
       </c>
       <c r="M23" s="1">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="N23" s="1">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="O23" s="1">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="P23" s="1">
         <v>0.06</v>
       </c>
       <c r="Q23" s="1">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="R23" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="U23" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="W23" s="1">
+        <v>1</v>
+      </c>
+      <c r="X23" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="Y23" s="1">
         <v>0.17</v>
       </c>
-      <c r="S23" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="T23" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="U23" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="V23" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="W23" s="1">
-        <v>1</v>
-      </c>
-      <c r="X23" s="1">
-        <v>0.33</v>
-      </c>
-      <c r="Y23" s="1">
-        <v>0.21</v>
-      </c>
       <c r="Z23" s="1">
-        <v>0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
@@ -2239,16 +2239,16 @@
         <v>-0.03</v>
       </c>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>-0.02</v>
       </c>
       <c r="D24" s="1">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="E24" s="1">
-        <v>-0.01</v>
+        <v>-0.03</v>
       </c>
       <c r="F24" s="1">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
         <v>-0.02</v>
@@ -2263,28 +2263,28 @@
         <v>-0.03</v>
       </c>
       <c r="K24" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="L24" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L24" s="1">
-        <v>-0.03</v>
-      </c>
       <c r="M24" s="1">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="N24" s="1">
         <v>-0.02</v>
       </c>
       <c r="O24" s="1">
-        <v>0.04</v>
+        <v>-0.02</v>
       </c>
       <c r="P24" s="1">
         <v>0.1</v>
       </c>
       <c r="Q24" s="1">
-        <v>-0.02</v>
+        <v>0.09</v>
       </c>
       <c r="R24" s="1">
-        <v>0.09</v>
+        <v>-0.02</v>
       </c>
       <c r="S24" s="1">
         <v>-0.01</v>
@@ -2296,10 +2296,10 @@
         <v>0.03</v>
       </c>
       <c r="V24" s="1">
-        <v>0.03</v>
+        <v>0.33</v>
       </c>
       <c r="W24" s="1">
-        <v>0.33</v>
+        <v>0.03</v>
       </c>
       <c r="X24" s="1">
         <v>1</v>
@@ -2322,13 +2322,13 @@
         <v>0</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="E25" s="1">
-        <v>-0.01</v>
+        <v>-0.05</v>
       </c>
       <c r="F25" s="1">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="G25" s="1">
         <v>-0.01</v>
@@ -2343,28 +2343,28 @@
         <v>-0.05</v>
       </c>
       <c r="K25" s="1">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="L25" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="M25" s="1">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="O25" s="1">
-        <v>0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="P25" s="1">
         <v>0.1</v>
       </c>
       <c r="Q25" s="1">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="R25" s="1">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="S25" s="1">
         <v>0.02</v>
@@ -2373,13 +2373,13 @@
         <v>0.09</v>
       </c>
       <c r="U25" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="V25" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="W25" s="1">
         <v>0.17</v>
-      </c>
-      <c r="V25" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="W25" s="1">
-        <v>0.21</v>
       </c>
       <c r="X25" s="1">
         <v>0.21</v>
@@ -2399,17 +2399,17 @@
         <v>0</v>
       </c>
       <c r="C26" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="D26" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
         <v>0.04</v>
       </c>
-      <c r="D26" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="E26" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="F26" s="1">
-        <v>0</v>
-      </c>
       <c r="G26" s="1">
         <v>-0.02</v>
       </c>
@@ -2423,16 +2423,16 @@
         <v>-0.02</v>
       </c>
       <c r="K26" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="L26" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L26" s="1">
-        <v>0</v>
-      </c>
       <c r="M26" s="1">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="N26" s="1">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="O26" s="1">
         <v>-0.01</v>
@@ -2441,10 +2441,10 @@
         <v>0.12</v>
       </c>
       <c r="Q26" s="1">
-        <v>-0.04</v>
+        <v>0.05</v>
       </c>
       <c r="R26" s="1">
-        <v>0.05</v>
+        <v>-0.04</v>
       </c>
       <c r="S26" s="1">
         <v>-0.02</v>
@@ -2453,13 +2453,13 @@
         <v>0.02</v>
       </c>
       <c r="U26" s="1">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
       <c r="V26" s="1">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
       <c r="W26" s="1">
-        <v>0.11</v>
+        <v>-0.01</v>
       </c>
       <c r="X26" s="1">
         <v>0.13</v>

</xml_diff>